<commit_message>
tests(test_urban_district_upscaling_source.py): add test for create_source method
</commit_message>
<xml_diff>
--- a/tests/standard_parameters.xlsx
+++ b/tests/standard_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/program_files/urban_district_upscaling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DFAB51-CD91-4949-B855-17D49705C8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475AF018-5058-DD41-8615-F6C6B57D9FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="5" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="311">
   <si>
     <t>start date</t>
   </si>
@@ -511,9 +511,6 @@
     <t>C2</t>
   </si>
   <si>
-    <t>Temperature Inlet</t>
-  </si>
-  <si>
     <t>Temperature Difference</t>
   </si>
   <si>
@@ -980,6 +977,9 @@
   </si>
   <si>
     <t>anergy_heat_pump</t>
+  </si>
+  <si>
+    <t>source_type</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1069,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1077,7 +1077,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1086,14 +1085,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 3" xfId="1" xr:uid="{3EB3DAA0-9F71-48CB-8FEA-1E1CAF40E04C}"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -1578,13 +1570,13 @@
         <v>92</v>
       </c>
       <c r="B1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1" t="s">
         <v>267</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>268</v>
-      </c>
-      <c r="D1" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3101,7 +3093,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B111">
         <v>0.35</v>
@@ -3115,7 +3107,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B112">
         <v>0.21</v>
@@ -3143,7 +3135,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B114">
         <v>7.14</v>
@@ -3171,7 +3163,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B116">
         <v>286</v>
@@ -3211,750 +3203,750 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="N1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>57.408200000000001</v>
+      </c>
+      <c r="F2" s="6">
+        <v>410770</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6">
+        <v>5046</v>
+      </c>
+      <c r="J2" s="6">
+        <v>57</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
         <v>295</v>
       </c>
-      <c r="B2" s="7">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="M2" s="6">
+        <v>1</v>
+      </c>
+      <c r="N2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>23.674199999999999</v>
+      </c>
+      <c r="F3" s="6">
+        <v>26112</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>611</v>
+      </c>
+      <c r="J3" s="6">
+        <v>24</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>295</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1</v>
+      </c>
+      <c r="N3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>39.284799999999997</v>
+      </c>
+      <c r="F4" s="6">
+        <v>8220</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>1174</v>
+      </c>
+      <c r="J4" s="6">
+        <v>39</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>295</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1</v>
+      </c>
+      <c r="N4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>18.648700000000002</v>
+      </c>
+      <c r="F5" s="6">
+        <v>8344</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>562</v>
+      </c>
+      <c r="J5" s="6">
+        <v>19</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>295</v>
+      </c>
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
+      <c r="N5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>31.479500000000002</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1490</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>774</v>
+      </c>
+      <c r="J6" s="6">
+        <v>31</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>295</v>
+      </c>
+      <c r="M6" s="6">
+        <v>1</v>
+      </c>
+      <c r="N6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>49.602899999999998</v>
+      </c>
+      <c r="F7" s="6">
+        <v>76830</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>2719</v>
+      </c>
+      <c r="J7" s="6">
+        <v>50</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>295</v>
+      </c>
+      <c r="M7" s="6">
+        <v>1</v>
+      </c>
+      <c r="N7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1.4E-5</v>
+      </c>
+      <c r="E8" s="6">
+        <v>31.479500000000002</v>
+      </c>
+      <c r="F8" s="6">
+        <v>99999</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.31030000000000002</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6">
+        <v>18084</v>
+      </c>
+      <c r="L8" t="s">
+        <v>295</v>
+      </c>
+      <c r="M8" s="6">
+        <v>1</v>
+      </c>
+      <c r="N8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>9999</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>8.7723999999999996E-2</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.62702500000000005</v>
+      </c>
+      <c r="L9" t="s">
+        <v>295</v>
+      </c>
+      <c r="M9" s="6">
+        <v>1</v>
+      </c>
+      <c r="N9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
         <v>57.408200000000001</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F10" s="6">
         <v>410770</v>
       </c>
-      <c r="G2" s="7">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7">
-        <v>0</v>
-      </c>
-      <c r="I2" s="7">
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
         <v>5046</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J10" s="6">
         <v>57</v>
       </c>
-      <c r="K2" s="7">
-        <v>0</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>303</v>
+      </c>
+      <c r="M10" s="6">
+        <v>1</v>
+      </c>
+      <c r="N10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="M2" s="7">
-        <v>1</v>
-      </c>
-      <c r="N2" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>23.674199999999999</v>
+      </c>
+      <c r="F11" s="6">
+        <v>26112</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>611</v>
+      </c>
+      <c r="J11" s="6">
+        <v>24</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>303</v>
+      </c>
+      <c r="M11" s="6">
+        <v>1</v>
+      </c>
+      <c r="N11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="B3" s="7">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7">
-        <v>23.674199999999999</v>
-      </c>
-      <c r="F3" s="7">
-        <v>26112</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0</v>
-      </c>
-      <c r="I3" s="7">
-        <v>611</v>
-      </c>
-      <c r="J3" s="7">
-        <v>24</v>
-      </c>
-      <c r="K3" s="7">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="M3" s="7">
-        <v>1</v>
-      </c>
-      <c r="N3" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>39.284799999999997</v>
+      </c>
+      <c r="F12" s="6">
+        <v>8220</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1174</v>
+      </c>
+      <c r="J12" s="6">
+        <v>39</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>303</v>
+      </c>
+      <c r="M12" s="6">
+        <v>1</v>
+      </c>
+      <c r="N12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7">
-        <v>39.284799999999997</v>
-      </c>
-      <c r="F4" s="7">
-        <v>8220</v>
-      </c>
-      <c r="G4" s="7">
-        <v>0</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0</v>
-      </c>
-      <c r="I4" s="7">
-        <v>1174</v>
-      </c>
-      <c r="J4" s="7">
-        <v>39</v>
-      </c>
-      <c r="K4" s="7">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="M4" s="7">
-        <v>1</v>
-      </c>
-      <c r="N4" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
+      <c r="E13" s="6">
+        <v>18.648700000000002</v>
+      </c>
+      <c r="F13" s="6">
+        <v>8344</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0</v>
+      </c>
+      <c r="I13" s="6">
+        <v>562</v>
+      </c>
+      <c r="J13" s="6">
+        <v>19</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>303</v>
+      </c>
+      <c r="M13" s="6">
+        <v>1</v>
+      </c>
+      <c r="N13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="B5" s="7">
-        <v>0</v>
-      </c>
-      <c r="C5" s="7">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7">
-        <v>18.648700000000002</v>
-      </c>
-      <c r="F5" s="7">
-        <v>8344</v>
-      </c>
-      <c r="G5" s="7">
-        <v>0</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0</v>
-      </c>
-      <c r="I5" s="7">
-        <v>562</v>
-      </c>
-      <c r="J5" s="7">
-        <v>19</v>
-      </c>
-      <c r="K5" s="7">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="M5" s="7">
-        <v>1</v>
-      </c>
-      <c r="N5" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>31.479500000000002</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1490</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <v>774</v>
+      </c>
+      <c r="J14" s="6">
+        <v>31</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>303</v>
+      </c>
+      <c r="M14" s="6">
+        <v>1</v>
+      </c>
+      <c r="N14" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="B6" s="7">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>49.602899999999998</v>
+      </c>
+      <c r="F15" s="6">
+        <v>76830</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6">
+        <v>2719</v>
+      </c>
+      <c r="J15" s="6">
+        <v>50</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>303</v>
+      </c>
+      <c r="M15" s="6">
+        <v>1</v>
+      </c>
+      <c r="N15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1.4E-5</v>
+      </c>
+      <c r="E16" s="6">
         <v>31.479500000000002</v>
       </c>
-      <c r="F6" s="7">
-        <v>1490</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0</v>
-      </c>
-      <c r="I6" s="7">
-        <v>774</v>
-      </c>
-      <c r="J6" s="7">
-        <v>31</v>
-      </c>
-      <c r="K6" s="7">
-        <v>0</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="M6" s="7">
-        <v>1</v>
-      </c>
-      <c r="N6" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="B7" s="7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7">
-        <v>49.602899999999998</v>
-      </c>
-      <c r="F7" s="7">
-        <v>76830</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="7">
-        <v>2719</v>
-      </c>
-      <c r="J7" s="7">
-        <v>50</v>
-      </c>
-      <c r="K7" s="7">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="M7" s="7">
-        <v>1</v>
-      </c>
-      <c r="N7" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="F16" s="6">
+        <v>99999</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.31030000000000002</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <v>0</v>
+      </c>
+      <c r="K16" s="6">
+        <v>18084</v>
+      </c>
+      <c r="L16" t="s">
+        <v>303</v>
+      </c>
+      <c r="M16" s="6">
+        <v>1</v>
+      </c>
+      <c r="N16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="B8" s="7">
-        <v>0</v>
-      </c>
-      <c r="C8" s="7">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7">
-        <v>1.4E-5</v>
-      </c>
-      <c r="E8" s="7">
-        <v>31.479500000000002</v>
-      </c>
-      <c r="F8" s="7">
-        <v>99999</v>
-      </c>
-      <c r="G8" s="7">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0.31030000000000002</v>
-      </c>
-      <c r="I8" s="7">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7">
-        <v>0</v>
-      </c>
-      <c r="K8" s="7">
-        <v>18084</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="M8" s="7">
-        <v>1</v>
-      </c>
-      <c r="N8" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6">
+        <v>9999</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>8.7723999999999996E-2</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0</v>
+      </c>
+      <c r="J17" s="6">
+        <v>0</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0.62702500000000005</v>
+      </c>
+      <c r="L17" t="s">
         <v>303</v>
       </c>
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7">
-        <v>0</v>
-      </c>
-      <c r="D9" s="7">
-        <v>2.1999999999999999E-5</v>
-      </c>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7">
-        <v>9999</v>
-      </c>
-      <c r="G9" s="7">
-        <v>0</v>
-      </c>
-      <c r="H9" s="7">
-        <v>8.7723999999999996E-2</v>
-      </c>
-      <c r="I9" s="7">
-        <v>0</v>
-      </c>
-      <c r="J9" s="7">
-        <v>0</v>
-      </c>
-      <c r="K9" s="7">
-        <v>0.62702500000000005</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="M9" s="7">
-        <v>1</v>
-      </c>
-      <c r="N9" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="B10" s="7">
-        <v>0</v>
-      </c>
-      <c r="C10" s="7">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7">
-        <v>57.408200000000001</v>
-      </c>
-      <c r="F10" s="7">
-        <v>410770</v>
-      </c>
-      <c r="G10" s="7">
-        <v>0</v>
-      </c>
-      <c r="H10" s="7">
-        <v>0</v>
-      </c>
-      <c r="I10" s="7">
-        <v>5046</v>
-      </c>
-      <c r="J10" s="7">
-        <v>57</v>
-      </c>
-      <c r="K10" s="7">
-        <v>0</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="M10" s="7">
-        <v>1</v>
-      </c>
-      <c r="N10" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="B11" s="7">
-        <v>0</v>
-      </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7">
-        <v>23.674199999999999</v>
-      </c>
-      <c r="F11" s="7">
-        <v>26112</v>
-      </c>
-      <c r="G11" s="7">
-        <v>0</v>
-      </c>
-      <c r="H11" s="7">
-        <v>0</v>
-      </c>
-      <c r="I11" s="7">
-        <v>611</v>
-      </c>
-      <c r="J11" s="7">
-        <v>24</v>
-      </c>
-      <c r="K11" s="7">
-        <v>0</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="M11" s="7">
-        <v>1</v>
-      </c>
-      <c r="N11" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="B12" s="7">
-        <v>0</v>
-      </c>
-      <c r="C12" s="7">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7">
-        <v>39.284799999999997</v>
-      </c>
-      <c r="F12" s="7">
-        <v>8220</v>
-      </c>
-      <c r="G12" s="7">
-        <v>0</v>
-      </c>
-      <c r="H12" s="7">
-        <v>0</v>
-      </c>
-      <c r="I12" s="7">
-        <v>1174</v>
-      </c>
-      <c r="J12" s="7">
-        <v>39</v>
-      </c>
-      <c r="K12" s="7">
-        <v>0</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="M12" s="7">
-        <v>1</v>
-      </c>
-      <c r="N12" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="B13" s="7">
-        <v>0</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
-      <c r="E13" s="7">
-        <v>18.648700000000002</v>
-      </c>
-      <c r="F13" s="7">
-        <v>8344</v>
-      </c>
-      <c r="G13" s="7">
-        <v>0</v>
-      </c>
-      <c r="H13" s="7">
-        <v>0</v>
-      </c>
-      <c r="I13" s="7">
-        <v>562</v>
-      </c>
-      <c r="J13" s="7">
-        <v>19</v>
-      </c>
-      <c r="K13" s="7">
-        <v>0</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="M13" s="7">
-        <v>1</v>
-      </c>
-      <c r="N13" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="B14" s="7">
-        <v>0</v>
-      </c>
-      <c r="C14" s="7">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7">
-        <v>31.479500000000002</v>
-      </c>
-      <c r="F14" s="7">
-        <v>1490</v>
-      </c>
-      <c r="G14" s="7">
-        <v>0</v>
-      </c>
-      <c r="H14" s="7">
-        <v>0</v>
-      </c>
-      <c r="I14" s="7">
-        <v>774</v>
-      </c>
-      <c r="J14" s="7">
-        <v>31</v>
-      </c>
-      <c r="K14" s="7">
-        <v>0</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="M14" s="7">
-        <v>1</v>
-      </c>
-      <c r="N14" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="B15" s="7">
-        <v>0</v>
-      </c>
-      <c r="C15" s="7">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7">
-        <v>49.602899999999998</v>
-      </c>
-      <c r="F15" s="7">
-        <v>76830</v>
-      </c>
-      <c r="G15" s="7">
-        <v>0</v>
-      </c>
-      <c r="H15" s="7">
-        <v>0</v>
-      </c>
-      <c r="I15" s="7">
-        <v>2719</v>
-      </c>
-      <c r="J15" s="7">
-        <v>50</v>
-      </c>
-      <c r="K15" s="7">
-        <v>0</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="M15" s="7">
-        <v>1</v>
-      </c>
-      <c r="N15" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="B16" s="7">
-        <v>0</v>
-      </c>
-      <c r="C16" s="7">
-        <v>0</v>
-      </c>
-      <c r="D16" s="7">
-        <v>1.4E-5</v>
-      </c>
-      <c r="E16" s="7">
-        <v>31.479500000000002</v>
-      </c>
-      <c r="F16" s="7">
-        <v>99999</v>
-      </c>
-      <c r="G16" s="7">
-        <v>0</v>
-      </c>
-      <c r="H16" s="7">
-        <v>0.31030000000000002</v>
-      </c>
-      <c r="I16" s="7">
-        <v>0</v>
-      </c>
-      <c r="J16" s="7">
-        <v>0</v>
-      </c>
-      <c r="K16" s="7">
-        <v>18084</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="M16" s="7">
-        <v>1</v>
-      </c>
-      <c r="N16" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="B17" s="7">
-        <v>1</v>
-      </c>
-      <c r="C17" s="7">
-        <v>0</v>
-      </c>
-      <c r="D17" s="7">
-        <v>2.1999999999999999E-5</v>
-      </c>
-      <c r="E17" s="7">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7">
-        <v>9999</v>
-      </c>
-      <c r="G17" s="7">
-        <v>0</v>
-      </c>
-      <c r="H17" s="7">
-        <v>8.7723999999999996E-2</v>
-      </c>
-      <c r="I17" s="7">
-        <v>0</v>
-      </c>
-      <c r="J17" s="7">
-        <v>0</v>
-      </c>
-      <c r="K17" s="7">
-        <v>0.62702500000000005</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="M17" s="7">
-        <v>1</v>
-      </c>
-      <c r="N17" s="7">
+      <c r="M17" s="6">
+        <v>1</v>
+      </c>
+      <c r="N17" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3982,82 +3974,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="6">
+        <v>0.15655827580000001</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.91229020000000005</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2.898939E-2</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="B2" s="7">
-        <v>0.15655827580000001</v>
-      </c>
-      <c r="C2" s="7">
-        <v>0.91229020000000005</v>
-      </c>
-      <c r="D2" s="7">
-        <v>2.898939E-2</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0</v>
-      </c>
-      <c r="F2" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="6">
+        <v>85</v>
+      </c>
+      <c r="C3" s="7">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.98</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>309</v>
       </c>
-      <c r="B3" s="7">
-        <v>85</v>
-      </c>
-      <c r="C3" s="8">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0.98</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>0</v>
       </c>
     </row>
@@ -4070,7 +4062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6075F4E-6449-42F6-B0A2-E3B463F49D3C}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -4198,7 +4190,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4227,7 +4219,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4256,7 +4248,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5039,17 +5031,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:I5 B9:I34 F6">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:I6">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:I8">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5063,7 +5055,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5106,7 +5098,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5135,7 +5127,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5164,7 +5156,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5193,7 +5185,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5860,7 +5852,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:I28">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13952,7 +13944,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:X110">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14164,7 +14156,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:U3">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14174,274 +14166,268 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865B2AF4-2CF4-4093-8D70-C931333F20A4}">
-  <dimension ref="A1:AF7"/>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A7"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>310</v>
       </c>
       <c r="B1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>132</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>133</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>134</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>135</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>136</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>137</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>138</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>139</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>140</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>141</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>142</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>143</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>144</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>145</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>146</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>147</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>148</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>149</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>150</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>151</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>152</v>
       </c>
-      <c r="Y1" t="s">
-        <v>153</v>
-      </c>
       <c r="Z1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA1" t="s">
         <v>154</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>155</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>156</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>157</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>158</v>
       </c>
-      <c r="AE1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AF1" t="s">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>162</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>27</v>
+      </c>
+      <c r="H3">
+        <v>95</v>
+      </c>
+      <c r="I3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
         <v>163</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>27</v>
-      </c>
-      <c r="G3">
-        <v>95</v>
-      </c>
-      <c r="H3">
+      <c r="M3" t="s">
+        <v>164</v>
+      </c>
+      <c r="N3" t="s">
+        <v>165</v>
+      </c>
+      <c r="O3" t="s">
+        <v>166</v>
+      </c>
+      <c r="P3">
+        <v>0.18</v>
+      </c>
+      <c r="Q3">
+        <v>75</v>
+      </c>
+      <c r="R3">
+        <v>0.19</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>75</v>
+      </c>
+      <c r="I4">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>164</v>
-      </c>
-      <c r="L3" t="s">
-        <v>165</v>
-      </c>
-      <c r="M3" t="s">
-        <v>166</v>
-      </c>
-      <c r="N3" t="s">
-        <v>167</v>
-      </c>
-      <c r="O3">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>0.18</v>
       </c>
-      <c r="P3">
+      <c r="Q4">
         <v>75</v>
       </c>
-      <c r="Q3">
-        <v>0.19</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>12</v>
-      </c>
-      <c r="G4">
-        <v>75</v>
-      </c>
-      <c r="H4">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0.18</v>
-      </c>
-      <c r="P4">
-        <v>75</v>
-      </c>
-      <c r="Q4">
+      <c r="R4">
         <v>0.78</v>
       </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
       <c r="S4">
         <v>0</v>
       </c>
@@ -14449,22 +14435,22 @@
         <v>0</v>
       </c>
       <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
         <v>0.78</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>3.8</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
       <c r="Y4">
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AA4">
         <v>10</v>
@@ -14481,261 +14467,252 @@
       <c r="AE4">
         <v>0</v>
       </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>170</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>27</v>
+      </c>
+      <c r="H5">
+        <v>95</v>
+      </c>
+      <c r="I5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>171</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>27</v>
       </c>
-      <c r="G5">
-        <v>95</v>
-      </c>
-      <c r="H5">
+      <c r="H6">
+        <v>71</v>
+      </c>
+      <c r="I6">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-      <c r="AC5">
-        <v>0</v>
-      </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5">
-        <v>0</v>
-      </c>
-      <c r="AF5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>163</v>
+      </c>
+      <c r="M6" t="s">
+        <v>164</v>
+      </c>
+      <c r="N6" t="s">
+        <v>165</v>
+      </c>
+      <c r="O6" t="s">
+        <v>166</v>
+      </c>
+      <c r="P6">
+        <v>0.18</v>
+      </c>
+      <c r="Q6">
+        <v>75</v>
+      </c>
+      <c r="R6">
+        <v>0.19</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>172</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>163</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>27</v>
-      </c>
-      <c r="G6">
-        <v>71</v>
-      </c>
-      <c r="H6">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>164</v>
-      </c>
-      <c r="L6" t="s">
-        <v>165</v>
-      </c>
-      <c r="M6" t="s">
-        <v>166</v>
-      </c>
-      <c r="N6" t="s">
-        <v>167</v>
-      </c>
-      <c r="O6">
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
         <v>0.18</v>
       </c>
-      <c r="P6">
+      <c r="Q7">
         <v>75</v>
       </c>
-      <c r="Q6">
-        <v>0.19</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>12</v>
-      </c>
-      <c r="G7">
-        <v>30</v>
-      </c>
-      <c r="H7">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0.18</v>
-      </c>
-      <c r="P7">
-        <v>75</v>
-      </c>
-      <c r="Q7">
+      <c r="R7">
         <v>0.78</v>
       </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
       <c r="S7">
         <v>0</v>
       </c>
@@ -14743,22 +14720,22 @@
         <v>0</v>
       </c>
       <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
         <v>0.78</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>3.8</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
       <c r="Y7">
         <v>0</v>
       </c>
       <c r="Z7">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AA7">
         <v>10</v>
@@ -14775,22 +14752,15 @@
       <c r="AE7">
         <v>0</v>
       </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:AF5">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6:AF7">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+  <conditionalFormatting sqref="B3:AE7">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -14816,40 +14786,40 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" t="s">
         <v>174</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>175</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>176</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>177</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>178</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>179</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>180</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>181</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>182</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>183</v>
       </c>
-      <c r="M1" t="s">
-        <v>184</v>
-      </c>
       <c r="N1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O1" t="s">
         <v>135</v>
@@ -14867,87 +14837,87 @@
         <v>138</v>
       </c>
       <c r="T1" t="s">
+        <v>184</v>
+      </c>
+      <c r="U1" t="s">
         <v>185</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>186</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>187</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>188</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>189</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>190</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>191</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>192</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>193</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>194</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>195</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>196</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>197</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>198</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>199</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>200</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>201</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>202</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>203</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>204</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>205</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>206</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>207</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>209</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>210</v>
       </c>
       <c r="D3">
         <v>0.375</v>
@@ -15072,13 +15042,13 @@
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D4">
         <v>0.39</v>
@@ -15203,13 +15173,13 @@
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D5">
         <v>0.92</v>
@@ -15334,13 +15304,13 @@
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>213</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>214</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -15391,10 +15361,10 @@
         <v>0</v>
       </c>
       <c r="T6" t="s">
+        <v>214</v>
+      </c>
+      <c r="U6" t="s">
         <v>215</v>
-      </c>
-      <c r="U6" t="s">
-        <v>216</v>
       </c>
       <c r="V6">
         <v>60</v>
@@ -15465,13 +15435,13 @@
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -15522,10 +15492,10 @@
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="V7">
         <v>60</v>
@@ -15596,13 +15566,13 @@
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -15653,10 +15623,10 @@
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="V8">
         <v>60</v>
@@ -15727,13 +15697,13 @@
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -15784,10 +15754,10 @@
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="V9">
         <v>60</v>
@@ -15858,13 +15828,13 @@
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -15989,13 +15959,13 @@
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D11">
         <v>0.78500000000000003</v>
@@ -16120,13 +16090,13 @@
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D12">
         <v>0.83</v>
@@ -16251,13 +16221,13 @@
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D13">
         <v>0.4</v>
@@ -16382,13 +16352,13 @@
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D14">
         <v>0.98</v>
@@ -16513,13 +16483,13 @@
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D15">
         <v>0.98</v>
@@ -16644,13 +16614,13 @@
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D16">
         <v>0.98</v>
@@ -16775,13 +16745,13 @@
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D17">
         <v>0.92</v>
@@ -16906,13 +16876,13 @@
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -16963,10 +16933,10 @@
         <v>0</v>
       </c>
       <c r="T18" t="s">
+        <v>214</v>
+      </c>
+      <c r="U18" t="s">
         <v>215</v>
-      </c>
-      <c r="U18" t="s">
-        <v>216</v>
       </c>
       <c r="V18">
         <v>60</v>
@@ -17037,13 +17007,13 @@
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D19">
         <v>0.35</v>
@@ -17168,13 +17138,13 @@
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D20">
         <v>0.35</v>
@@ -17299,13 +17269,13 @@
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D21">
         <v>0.92</v>
@@ -17430,13 +17400,13 @@
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D22">
         <v>0.9</v>
@@ -17561,13 +17531,13 @@
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D23">
         <v>0.89</v>
@@ -17692,13 +17662,13 @@
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D24">
         <v>0.92</v>
@@ -17836,12 +17806,12 @@
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
@@ -17852,16 +17822,16 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" t="s">
         <v>183</v>
       </c>
-      <c r="E1" t="s">
-        <v>184</v>
-      </c>
       <c r="F1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G1" t="s">
         <v>135</v>
@@ -17879,63 +17849,63 @@
         <v>138</v>
       </c>
       <c r="L1" t="s">
+        <v>236</v>
+      </c>
+      <c r="M1" t="s">
         <v>237</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>238</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>239</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>240</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>241</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>242</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>243</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
+        <v>176</v>
+      </c>
+      <c r="U1" t="s">
+        <v>177</v>
+      </c>
+      <c r="V1" t="s">
+        <v>179</v>
+      </c>
+      <c r="W1" t="s">
+        <v>180</v>
+      </c>
+      <c r="X1" t="s">
         <v>244</v>
       </c>
-      <c r="T1" t="s">
-        <v>177</v>
-      </c>
-      <c r="U1" t="s">
-        <v>178</v>
-      </c>
-      <c r="V1" t="s">
-        <v>180</v>
-      </c>
-      <c r="W1" t="s">
-        <v>181</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AA1" t="s">
         <v>245</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>187</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>247</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>248</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -18012,13 +17982,13 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -18095,13 +18065,13 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -18178,13 +18148,13 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -18261,13 +18231,13 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -18344,13 +18314,13 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -18447,7 +18417,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" t="s">
         <v>131</v>
@@ -18456,25 +18426,25 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" t="s">
         <v>183</v>
       </c>
-      <c r="I1" t="s">
-        <v>184</v>
-      </c>
       <c r="J1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K1" t="s">
         <v>135</v>
@@ -18494,16 +18464,16 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" t="s">
         <v>256</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>257</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>258</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -18541,16 +18511,16 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>257</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>258</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -18588,16 +18558,16 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>257</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>258</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -18635,16 +18605,16 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B6" t="s">
+        <v>256</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>257</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>258</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -18682,16 +18652,16 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>257</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>258</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -18729,16 +18699,16 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>257</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>258</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -18776,16 +18746,16 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>257</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>258</v>
       </c>
       <c r="E9">
         <v>0.9</v>
@@ -18823,16 +18793,16 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>257</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>258</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -18870,16 +18840,16 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B11" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>257</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>258</v>
       </c>
       <c r="E11">
         <v>1</v>

</xml_diff>

<commit_message>
code(US-Tool Sources): move existing capacity and min. investment into the standard parameters
</commit_message>
<xml_diff>
--- a/tests/standard_parameters.xlsx
+++ b/tests/standard_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475AF018-5058-DD41-8615-F6C6B57D9FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59165F82-79B0-F343-86E4-C393AD3B142D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="5" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="311">
   <si>
     <t>start date</t>
   </si>
@@ -14166,10 +14166,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865B2AF4-2CF4-4093-8D70-C931333F20A4}">
-  <dimension ref="A1:AE7"/>
+  <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AJ5" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14178,7 +14178,7 @@
     <col min="5" max="5" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>310</v>
       </c>
@@ -14272,13 +14272,19 @@
       <c r="AE1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -14372,8 +14378,14 @@
       <c r="AE3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>167</v>
       </c>
@@ -14467,8 +14479,14 @@
       <c r="AE4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>169</v>
       </c>
@@ -14562,8 +14580,14 @@
       <c r="AE5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>171</v>
       </c>
@@ -14657,8 +14681,14 @@
       <c r="AE6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>172</v>
       </c>
@@ -14752,9 +14782,15 @@
       <c r="AE7">
         <v>0</v>
       </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:AE7">
+  <conditionalFormatting sqref="B3:AG7">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
tests(test_urban_district_upscaling_storage): add test for building storages
</commit_message>
<xml_diff>
--- a/tests/standard_parameters.xlsx
+++ b/tests/standard_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59165F82-79B0-F343-86E4-C393AD3B142D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F03503E-E84A-5B41-B70D-E0CE6029B2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="5" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="7" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="312">
   <si>
     <t>start date</t>
   </si>
@@ -980,6 +980,9 @@
   </si>
   <si>
     <t>source_type</t>
+  </si>
+  <si>
+    <t>storage_type</t>
   </si>
 </sst>
 </file>
@@ -14168,7 +14171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865B2AF4-2CF4-4093-8D70-C931333F20A4}">
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="AJ5" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
@@ -17841,9 +17844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062F9C9F-EC6B-45A0-B400-3E864B701D31}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17852,7 +17853,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
tests(test_urban_district_upscaling_transformer): add test for create transformer
</commit_message>
<xml_diff>
--- a/tests/standard_parameters.xlsx
+++ b/tests/standard_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F03503E-E84A-5B41-B70D-E0CE6029B2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B08EC0E-89C7-DF40-9369-5E9F2703DA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="7" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="6" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="313">
   <si>
     <t>start date</t>
   </si>
@@ -983,6 +983,9 @@
   </si>
   <si>
     <t>storage_type</t>
+  </si>
+  <si>
+    <t>transformer_type</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1075,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1083,6 +1086,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3180,7 +3184,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D116">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14805,21 +14809,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB4EA7-D669-4B1E-9B4E-C2CB3560F5F3}">
-  <dimension ref="A1:AQ24"/>
+  <dimension ref="A1:AP24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="30" max="30" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>312</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -14882,73 +14887,70 @@
         <v>185</v>
       </c>
       <c r="V1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="X1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Y1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="Z1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AA1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AB1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AC1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AD1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AE1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AF1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AG1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AH1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AI1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AJ1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AK1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AL1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AM1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AN1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AO1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AP1" t="s">
-        <v>206</v>
-      </c>
-      <c r="AQ1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>208</v>
       </c>
@@ -15006,11 +15008,11 @@
       <c r="S3">
         <v>0</v>
       </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
+      <c r="T3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -15075,11 +15077,8 @@
       <c r="AP3">
         <v>0</v>
       </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>210</v>
       </c>
@@ -15137,11 +15136,11 @@
       <c r="S4">
         <v>0</v>
       </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
+      <c r="T4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -15206,11 +15205,8 @@
       <c r="AP4">
         <v>0</v>
       </c>
-      <c r="AQ4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>211</v>
       </c>
@@ -15268,11 +15264,11 @@
       <c r="S5">
         <v>0</v>
       </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
+      <c r="T5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -15337,11 +15333,8 @@
       <c r="AP5">
         <v>0</v>
       </c>
-      <c r="AQ5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>212</v>
       </c>
@@ -15399,29 +15392,29 @@
       <c r="S6">
         <v>0</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="8" t="s">
         <v>214</v>
       </c>
       <c r="U6" t="s">
         <v>215</v>
       </c>
       <c r="V6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X6">
-        <v>0.55000000000000004</v>
+        <v>100</v>
       </c>
       <c r="Y6">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="Z6">
         <v>100</v>
       </c>
-      <c r="Z6">
-        <v>3.2800000000000003E-2</v>
-      </c>
       <c r="AA6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AB6">
         <v>0</v>
@@ -15468,11 +15461,8 @@
       <c r="AP6">
         <v>0</v>
       </c>
-      <c r="AQ6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>216</v>
       </c>
@@ -15530,20 +15520,20 @@
       <c r="S7">
         <v>0</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="8" t="s">
         <v>214</v>
       </c>
       <c r="U7" t="s">
         <v>217</v>
       </c>
       <c r="V7">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="X7">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="Y7">
         <v>0</v>
@@ -15552,13 +15542,13 @@
         <v>0</v>
       </c>
       <c r="AA7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB7">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="AC7">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AD7">
         <v>0</v>
@@ -15599,11 +15589,8 @@
       <c r="AP7">
         <v>0</v>
       </c>
-      <c r="AQ7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>218</v>
       </c>
@@ -15661,20 +15648,20 @@
       <c r="S8">
         <v>0</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" s="8" t="s">
         <v>214</v>
       </c>
       <c r="U8" t="s">
         <v>219</v>
       </c>
       <c r="V8">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Y8">
         <v>0</v>
@@ -15730,11 +15717,8 @@
       <c r="AP8">
         <v>0</v>
       </c>
-      <c r="AQ8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>220</v>
       </c>
@@ -15792,20 +15776,20 @@
       <c r="S9">
         <v>0</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="8" t="s">
         <v>214</v>
       </c>
       <c r="U9" t="s">
         <v>217</v>
       </c>
       <c r="V9">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="X9">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -15814,13 +15798,13 @@
         <v>0</v>
       </c>
       <c r="AA9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB9">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="AC9">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AD9">
         <v>0</v>
@@ -15861,11 +15845,8 @@
       <c r="AP9">
         <v>0</v>
       </c>
-      <c r="AQ9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>221</v>
       </c>
@@ -15923,11 +15904,11 @@
       <c r="S10">
         <v>0</v>
       </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
+      <c r="T10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U10" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -15992,11 +15973,8 @@
       <c r="AP10">
         <v>0</v>
       </c>
-      <c r="AQ10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>222</v>
       </c>
@@ -16054,11 +16032,11 @@
       <c r="S11">
         <v>0</v>
       </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
+      <c r="T11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -16123,11 +16101,8 @@
       <c r="AP11">
         <v>0</v>
       </c>
-      <c r="AQ11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>223</v>
       </c>
@@ -16185,11 +16160,11 @@
       <c r="S12">
         <v>0</v>
       </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
+      <c r="T12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U12" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V12">
         <v>0</v>
@@ -16254,11 +16229,8 @@
       <c r="AP12">
         <v>0</v>
       </c>
-      <c r="AQ12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>224</v>
       </c>
@@ -16316,11 +16288,11 @@
       <c r="S13">
         <v>0</v>
       </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
+      <c r="T13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U13" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -16385,11 +16357,8 @@
       <c r="AP13">
         <v>0</v>
       </c>
-      <c r="AQ13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>225</v>
       </c>
@@ -16447,11 +16416,11 @@
       <c r="S14">
         <v>0</v>
       </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>0</v>
+      <c r="T14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U14" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V14">
         <v>0</v>
@@ -16516,11 +16485,8 @@
       <c r="AP14">
         <v>0</v>
       </c>
-      <c r="AQ14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>226</v>
       </c>
@@ -16578,11 +16544,11 @@
       <c r="S15">
         <v>0</v>
       </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
+      <c r="T15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U15" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -16647,11 +16613,8 @@
       <c r="AP15">
         <v>0</v>
       </c>
-      <c r="AQ15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>227</v>
       </c>
@@ -16709,11 +16672,11 @@
       <c r="S16">
         <v>0</v>
       </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
+      <c r="T16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U16" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V16">
         <v>0</v>
@@ -16778,11 +16741,8 @@
       <c r="AP16">
         <v>0</v>
       </c>
-      <c r="AQ16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>228</v>
       </c>
@@ -16840,11 +16800,11 @@
       <c r="S17">
         <v>0</v>
       </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
+      <c r="T17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U17" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -16909,11 +16869,8 @@
       <c r="AP17">
         <v>0</v>
       </c>
-      <c r="AQ17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>229</v>
       </c>
@@ -16971,29 +16928,29 @@
       <c r="S18">
         <v>0</v>
       </c>
-      <c r="T18" t="s">
+      <c r="T18" s="8" t="s">
         <v>214</v>
       </c>
       <c r="U18" t="s">
         <v>215</v>
       </c>
       <c r="V18">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="W18">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X18">
-        <v>0.55000000000000004</v>
+        <v>100</v>
       </c>
       <c r="Y18">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="Z18">
         <v>100</v>
       </c>
-      <c r="Z18">
-        <v>3.2800000000000003E-2</v>
-      </c>
       <c r="AA18">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AB18">
         <v>0</v>
@@ -17040,11 +16997,8 @@
       <c r="AP18">
         <v>0</v>
       </c>
-      <c r="AQ18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>230</v>
       </c>
@@ -17102,11 +17056,11 @@
       <c r="S19">
         <v>0</v>
       </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
+      <c r="T19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U19" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V19">
         <v>0</v>
@@ -17171,11 +17125,8 @@
       <c r="AP19">
         <v>0</v>
       </c>
-      <c r="AQ19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>231</v>
       </c>
@@ -17233,11 +17184,11 @@
       <c r="S20">
         <v>0</v>
       </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
+      <c r="T20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U20" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V20">
         <v>0</v>
@@ -17302,11 +17253,8 @@
       <c r="AP20">
         <v>0</v>
       </c>
-      <c r="AQ20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>232</v>
       </c>
@@ -17364,11 +17312,11 @@
       <c r="S21">
         <v>0</v>
       </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
+      <c r="T21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U21" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V21">
         <v>0</v>
@@ -17433,11 +17381,8 @@
       <c r="AP21">
         <v>0</v>
       </c>
-      <c r="AQ21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>233</v>
       </c>
@@ -17495,11 +17440,11 @@
       <c r="S22">
         <v>0</v>
       </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
+      <c r="T22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U22" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V22">
         <v>0</v>
@@ -17564,11 +17509,8 @@
       <c r="AP22">
         <v>0</v>
       </c>
-      <c r="AQ22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>234</v>
       </c>
@@ -17626,11 +17568,11 @@
       <c r="S23">
         <v>0</v>
       </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <v>0</v>
+      <c r="T23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U23" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V23">
         <v>0</v>
@@ -17695,11 +17637,8 @@
       <c r="AP23">
         <v>0</v>
       </c>
-      <c r="AQ23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>273</v>
       </c>
@@ -17757,11 +17696,11 @@
       <c r="S24">
         <v>0</v>
       </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <v>0</v>
+      <c r="T24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U24" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="V24">
         <v>0</v>
@@ -17826,13 +17765,10 @@
       <c r="AP24">
         <v>0</v>
       </c>
-      <c r="AQ24">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:AQ24">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="B3:AP24">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17844,7 +17780,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062F9C9F-EC6B-45A0-B400-3E864B701D31}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18434,7 +18372,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:AA8">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18924,7 +18862,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:O11">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
tests(preprocessing): add empty test methods that have to be filled later
</commit_message>
<xml_diff>
--- a/tests/standard_parameters.xlsx
+++ b/tests/standard_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B08EC0E-89C7-DF40-9369-5E9F2703DA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5FF366-345E-974A-9E23-4F14BB37B260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="6" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="9" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -1563,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0876A1A-D601-4F49-AE30-77EB630A1DC1}">
   <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14811,7 +14811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB4EA7-D669-4B1E-9B4E-C2CB3560F5F3}">
   <dimension ref="A1:AP24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
tests(test_urban_district_upscaling_central_components): test create central chp
</commit_message>
<xml_diff>
--- a/tests/standard_parameters.xlsx
+++ b/tests/standard_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6FF7A9-0D17-F94F-B040-5D16C9AA0640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E514C540-977D-C542-A29D-00D9969C99AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23600" windowHeight="16400" activeTab="1" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23600" windowHeight="16400" activeTab="8" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="319">
   <si>
     <t>start date</t>
   </si>
@@ -995,6 +995,15 @@
   </si>
   <si>
     <t>central_pellet_building_link</t>
+  </si>
+  <si>
+    <t>central_biogas_chp_link</t>
+  </si>
+  <si>
+    <t>central_woodchips_chp_link</t>
+  </si>
+  <si>
+    <t>central_pellet_chp_link</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1111,42 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 3" xfId="1" xr:uid="{3EB3DAA0-9F71-48CB-8FEA-1E1CAF40E04C}"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3215,7 +3259,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D116">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4100,7 +4144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6075F4E-6449-42F6-B0A2-E3B463F49D3C}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I34"/>
     </sheetView>
   </sheetViews>
@@ -5072,17 +5116,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:I5 B9:I34 F6">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:I6">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:I8">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5893,7 +5937,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:I28">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13985,7 +14029,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:X110">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14197,7 +14241,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:U3">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14832,7 +14876,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AG7">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14845,8 +14889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB4EA7-D669-4B1E-9B4E-C2CB3560F5F3}">
   <dimension ref="A1:AP24"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17802,7 +17846,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AP24">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18406,7 +18450,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:AA8">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18416,10 +18460,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F7A117-64AB-4955-A232-50A2E399D809}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19038,23 +19082,179 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>316</v>
+      </c>
+      <c r="B15" t="s">
+        <v>256</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>257</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>9999</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L15">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>317</v>
+      </c>
+      <c r="B16" t="s">
+        <v>256</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>257</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>9999</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>318</v>
+      </c>
+      <c r="B17" t="s">
+        <v>256</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>257</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>9999</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L17">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A3:O11">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:O12">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:O13">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:O14">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:O15">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13:O13">
+  <conditionalFormatting sqref="A16:O16">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:O14">
+  <conditionalFormatting sqref="A17:O17">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
tests(US-Tool): add new test
</commit_message>
<xml_diff>
--- a/tests/standard_parameters.xlsx
+++ b/tests/standard_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C443FCA-27F2-0C45-BA14-603CD5D486AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4E9389-CC0E-D14B-82E5-654296E3949C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="8" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="1" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="332">
   <si>
     <t>start date</t>
   </si>
@@ -1036,6 +1036,12 @@
   </si>
   <si>
     <t>cluster_electricity_link</t>
+  </si>
+  <si>
+    <t>central_h2_heat_link</t>
+  </si>
+  <si>
+    <t>central_h2_heat_bus</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1183,21 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 3" xfId="1" xr:uid="{3EB3DAA0-9F71-48CB-8FEA-1E1CAF40E04C}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3297,7 +3317,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D116">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4519,12 +4539,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4534,10 +4554,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6075F4E-6449-42F6-B0A2-E3B463F49D3C}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5093,13 +5113,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>331</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -5119,7 +5139,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -5128,24 +5148,24 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0.16539999999999999</v>
+        <v>0</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>366</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -5160,36 +5180,36 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>2.53E-2</v>
+        <v>0.16539999999999999</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>366</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>-5.1459999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>2.53E-2</v>
       </c>
       <c r="G26">
-        <v>-27</v>
+        <v>0</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -5197,129 +5217,129 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>-5.1459999999999999E-2</v>
       </c>
       <c r="F27">
-        <v>9.4500000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>-27</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>-0.128</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>-0.128</v>
       </c>
       <c r="F29">
-        <v>2.9000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>-0.128</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>-0.128</v>
       </c>
       <c r="F31">
-        <v>2.53E-2</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -5327,7 +5347,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5342,7 +5362,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>9.7000000000000003E-2</v>
+        <v>2.53E-2</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -5353,7 +5373,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5368,7 +5388,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>9.4500000000000001E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -5379,43 +5399,69 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>9.4500000000000001E-2</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>47</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:H5 B9:H34 F6">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+  <conditionalFormatting sqref="B3:H5 B9:H22 F6 B24:H35">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:H6">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:H8">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6371,7 +6417,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:I26 B31:I32">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15153,12 +15199,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:N110">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:Z110">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15388,7 +15434,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:W3">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16023,7 +16069,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AG7">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16037,7 +16083,7 @@
   <dimension ref="A1:AP24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18993,7 +19039,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AP24">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19597,7 +19643,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:AA8">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19607,10 +19653,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F7A117-64AB-4955-A232-50A2E399D809}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20410,14 +20456,68 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>330</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>254</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>9999</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K20">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A3:N18">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:N19">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:C20">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20:N20">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
tests(US-Tool): fix tests after last commit made them crash
</commit_message>
<xml_diff>
--- a/tests/standard_parameters.xlsx
+++ b/tests/standard_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4E9389-CC0E-D14B-82E5-654296E3949C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F314A0-1C53-C843-9696-5AE39684CF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="1" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="6" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="331">
   <si>
     <t>start date</t>
   </si>
@@ -607,9 +607,6 @@
   </si>
   <si>
     <t>quality grade</t>
-  </si>
-  <si>
-    <t>length of the geoth. probe</t>
   </si>
   <si>
     <t>heat extraction</t>
@@ -1710,13 +1707,13 @@
         <v>91</v>
       </c>
       <c r="B1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C1" t="s">
         <v>263</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>264</v>
-      </c>
-      <c r="D1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3233,7 +3230,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B111">
         <v>0.35</v>
@@ -3247,7 +3244,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B112">
         <v>0.21</v>
@@ -3275,7 +3272,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B114">
         <v>7.14</v>
@@ -3303,7 +3300,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B116">
         <v>286</v>
@@ -3348,19 +3345,19 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>280</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>281</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>181</v>
@@ -3381,13 +3378,13 @@
         <v>136</v>
       </c>
       <c r="L1" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>283</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>284</v>
       </c>
       <c r="O1" t="s">
         <v>172</v>
@@ -3411,7 +3408,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B3" s="8">
         <v>0</v>
@@ -3444,7 +3441,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M3" s="8">
         <v>1</v>
@@ -3458,7 +3455,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B4" s="8">
         <v>0</v>
@@ -3491,7 +3488,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M4" s="8">
         <v>1</v>
@@ -3505,7 +3502,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B5" s="8">
         <v>0</v>
@@ -3538,7 +3535,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M5" s="8">
         <v>1</v>
@@ -3552,7 +3549,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B6" s="8">
         <v>0</v>
@@ -3585,7 +3582,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M6" s="8">
         <v>1</v>
@@ -3599,7 +3596,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -3632,7 +3629,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M7" s="8">
         <v>1</v>
@@ -3646,7 +3643,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -3679,7 +3676,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M8" s="8">
         <v>0</v>
@@ -3693,7 +3690,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B9" s="8">
         <v>0</v>
@@ -3726,7 +3723,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M9" s="8">
         <v>1</v>
@@ -3740,7 +3737,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B10" s="8">
         <v>0</v>
@@ -3773,7 +3770,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M10" s="8">
         <v>1</v>
@@ -3787,7 +3784,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B11" s="8">
         <v>0</v>
@@ -3820,7 +3817,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M11" s="8">
         <v>1</v>
@@ -3834,7 +3831,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B12" s="8">
         <v>0</v>
@@ -3867,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M12" s="8">
         <v>1</v>
@@ -3881,7 +3878,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B13" s="8">
         <v>0</v>
@@ -3914,7 +3911,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M13" s="8">
         <v>1</v>
@@ -3928,7 +3925,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B14" s="8">
         <v>0</v>
@@ -3961,7 +3958,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M14" s="8">
         <v>1</v>
@@ -3975,7 +3972,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B15" s="8">
         <v>1</v>
@@ -4008,7 +4005,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M15" s="8">
         <v>1</v>
@@ -4022,7 +4019,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B16" s="8">
         <v>0</v>
@@ -4055,7 +4052,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M16" s="8">
         <v>1</v>
@@ -4069,7 +4066,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B17" s="8">
         <v>0</v>
@@ -4102,7 +4099,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M17" s="8">
         <v>1</v>
@@ -4116,7 +4113,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B18" s="8">
         <v>0</v>
@@ -4149,7 +4146,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M18" s="8">
         <v>1</v>
@@ -4163,7 +4160,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B19" s="8">
         <v>0</v>
@@ -4196,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M19" s="8">
         <v>1</v>
@@ -4210,7 +4207,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B20" s="8">
         <v>0</v>
@@ -4243,7 +4240,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M20" s="8">
         <v>1</v>
@@ -4257,7 +4254,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B21" s="8">
         <v>0</v>
@@ -4290,7 +4287,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M21" s="8">
         <v>1</v>
@@ -4304,7 +4301,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B22" s="8">
         <v>0</v>
@@ -4337,7 +4334,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M22" s="8">
         <v>1</v>
@@ -4351,7 +4348,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -4384,7 +4381,7 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -4398,7 +4395,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4445,7 +4442,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -4492,7 +4489,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4556,7 +4553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6075F4E-6449-42F6-B0A2-E3B463F49D3C}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
@@ -4671,7 +4668,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4697,7 +4694,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4723,7 +4720,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5113,7 +5110,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -5518,7 +5515,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5547,7 +5544,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5576,7 +5573,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5605,7 +5602,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -6214,7 +6211,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B27" s="8">
         <v>1</v>
@@ -6243,7 +6240,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B28" s="8">
         <v>1</v>
@@ -6272,7 +6269,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B29" s="8">
         <v>1</v>
@@ -6301,16 +6298,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B30" s="8">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>327</v>
-      </c>
-      <c r="B30" s="8">
-        <v>1</v>
-      </c>
-      <c r="C30" s="8">
-        <v>1</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>328</v>
       </c>
       <c r="E30" s="11">
         <v>0</v>
@@ -6388,7 +6385,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B33" s="8">
         <v>1</v>
@@ -6509,52 +6506,52 @@
         <v>113</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>114</v>
       </c>
       <c r="Z1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="O2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Q2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="R2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="S2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="T2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="U2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="V2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="W2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="X2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Y2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Z2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -15287,10 +15284,10 @@
         <v>114</v>
       </c>
       <c r="V1" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="W1" t="s">
         <v>321</v>
-      </c>
-      <c r="W1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -15458,7 +15455,7 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B1" t="s">
         <v>157</v>
@@ -16080,22 +16077,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB4EA7-D669-4B1E-9B4E-C2CB3560F5F3}">
-  <dimension ref="A1:AP24"/>
+  <dimension ref="A1:AO24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
-    <col min="30" max="30" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -16217,19 +16214,16 @@
       <c r="AO1" t="s">
         <v>204</v>
       </c>
-      <c r="AP1" t="s">
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>206</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>207</v>
       </c>
       <c r="D3">
         <v>0.375</v>
@@ -16345,19 +16339,16 @@
       <c r="AO3">
         <v>0</v>
       </c>
-      <c r="AP3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D4">
         <v>0.39</v>
@@ -16473,19 +16464,16 @@
       <c r="AO4">
         <v>0</v>
       </c>
-      <c r="AP4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D5">
         <v>0.92</v>
@@ -16601,19 +16589,16 @@
       <c r="AO5">
         <v>0</v>
       </c>
-      <c r="AP5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>210</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>211</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -16664,10 +16649,10 @@
         <v>0</v>
       </c>
       <c r="T6" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="U6" t="s">
         <v>212</v>
-      </c>
-      <c r="U6" t="s">
-        <v>213</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -16676,13 +16661,13 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="X6">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="Y6">
         <v>100</v>
       </c>
-      <c r="Y6">
-        <v>3.2800000000000003E-2</v>
-      </c>
       <c r="Z6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AA6">
         <v>0</v>
@@ -16729,19 +16714,16 @@
       <c r="AO6">
         <v>0</v>
       </c>
-      <c r="AP6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -16792,10 +16774,10 @@
         <v>0</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="U7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -16810,13 +16792,13 @@
         <v>0</v>
       </c>
       <c r="Z7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA7">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="AB7">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -16857,19 +16839,16 @@
       <c r="AO7">
         <v>0</v>
       </c>
-      <c r="AP7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -16920,10 +16899,10 @@
         <v>0</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="U8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -16985,19 +16964,16 @@
       <c r="AO8">
         <v>0</v>
       </c>
-      <c r="AP8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -17048,10 +17024,10 @@
         <v>0</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="U9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -17066,13 +17042,13 @@
         <v>0</v>
       </c>
       <c r="Z9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA9">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="AB9">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -17113,19 +17089,16 @@
       <c r="AO9">
         <v>0</v>
       </c>
-      <c r="AP9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -17241,19 +17214,16 @@
       <c r="AO10">
         <v>0</v>
       </c>
-      <c r="AP10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D11">
         <v>0.78500000000000003</v>
@@ -17369,19 +17339,16 @@
       <c r="AO11">
         <v>0</v>
       </c>
-      <c r="AP11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D12">
         <v>0.83</v>
@@ -17497,19 +17464,16 @@
       <c r="AO12">
         <v>0</v>
       </c>
-      <c r="AP12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D13">
         <v>0.4</v>
@@ -17625,19 +17589,16 @@
       <c r="AO13">
         <v>0</v>
       </c>
-      <c r="AP13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D14">
         <v>0.98</v>
@@ -17753,19 +17714,16 @@
       <c r="AO14">
         <v>0</v>
       </c>
-      <c r="AP14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D15">
         <v>0.98</v>
@@ -17881,19 +17839,16 @@
       <c r="AO15">
         <v>0</v>
       </c>
-      <c r="AP15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D16">
         <v>0.98</v>
@@ -18009,19 +17964,16 @@
       <c r="AO16">
         <v>0</v>
       </c>
-      <c r="AP16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D17">
         <v>0.92</v>
@@ -18137,19 +18089,16 @@
       <c r="AO17">
         <v>0</v>
       </c>
-      <c r="AP17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -18200,10 +18149,10 @@
         <v>0</v>
       </c>
       <c r="T18" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="U18" t="s">
         <v>212</v>
-      </c>
-      <c r="U18" t="s">
-        <v>213</v>
       </c>
       <c r="V18">
         <v>0</v>
@@ -18212,13 +18161,13 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="X18">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="Y18">
         <v>100</v>
       </c>
-      <c r="Y18">
-        <v>3.2800000000000003E-2</v>
-      </c>
       <c r="Z18">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AA18">
         <v>0</v>
@@ -18265,19 +18214,16 @@
       <c r="AO18">
         <v>0</v>
       </c>
-      <c r="AP18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D19">
         <v>0.35</v>
@@ -18393,19 +18339,16 @@
       <c r="AO19">
         <v>0</v>
       </c>
-      <c r="AP19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D20">
         <v>0.35</v>
@@ -18521,19 +18464,16 @@
       <c r="AO20">
         <v>0</v>
       </c>
-      <c r="AP20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D21">
         <v>0.92</v>
@@ -18649,19 +18589,16 @@
       <c r="AO21">
         <v>0</v>
       </c>
-      <c r="AP21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D22">
         <v>0.9</v>
@@ -18777,19 +18714,16 @@
       <c r="AO22">
         <v>0</v>
       </c>
-      <c r="AP22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D23">
         <v>0.89</v>
@@ -18905,19 +18839,16 @@
       <c r="AO23">
         <v>0</v>
       </c>
-      <c r="AP23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D24">
         <v>0.92</v>
@@ -19033,12 +18964,9 @@
       <c r="AO24">
         <v>0</v>
       </c>
-      <c r="AP24">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:AP24">
+  <conditionalFormatting sqref="B3:AO24">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -19062,13 +18990,13 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D1" t="s">
         <v>180</v>
@@ -19095,28 +19023,28 @@
         <v>136</v>
       </c>
       <c r="L1" t="s">
+        <v>233</v>
+      </c>
+      <c r="M1" t="s">
         <v>234</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>235</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>236</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>237</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>238</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>239</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>240</v>
-      </c>
-      <c r="S1" t="s">
-        <v>241</v>
       </c>
       <c r="T1" t="s">
         <v>174</v>
@@ -19131,7 +19059,7 @@
         <v>178</v>
       </c>
       <c r="X1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Y1" t="s">
         <v>184</v>
@@ -19140,18 +19068,18 @@
         <v>185</v>
       </c>
       <c r="AA1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>244</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>245</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -19228,13 +19156,13 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -19311,13 +19239,13 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -19394,13 +19322,13 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -19477,13 +19405,13 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -19560,13 +19488,13 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -19666,13 +19594,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D1" t="s">
         <v>172</v>
@@ -19710,13 +19638,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>253</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>254</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -19754,13 +19682,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -19798,13 +19726,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -19842,13 +19770,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -19886,13 +19814,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -19930,13 +19858,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -19974,13 +19902,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -20018,13 +19946,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D10">
         <v>0.9</v>
@@ -20062,13 +19990,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -20106,13 +20034,13 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -20150,13 +20078,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -20194,13 +20122,13 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -20238,13 +20166,13 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -20282,13 +20210,13 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -20326,13 +20254,13 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -20370,13 +20298,13 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -20414,13 +20342,13 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -20458,13 +20386,13 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D20">
         <v>1</v>

</xml_diff>

<commit_message>
tests(): fix the unit tests to fit the new pandas structure
</commit_message>
<xml_diff>
--- a/tests/standard_parameters.xlsx
+++ b/tests/standard_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60806175-3223-3C47-A455-1E7B2484D799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551DCBF1-4063-8949-964D-1A1575146429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="6" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="1" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="329">
   <si>
     <t>start date</t>
   </si>
@@ -520,9 +520,6 @@
   </si>
   <si>
     <t>max. investment capacity</t>
-  </si>
-  <si>
-    <t>units</t>
   </si>
   <si>
     <t>fixed photovoltaic source</t>
@@ -1177,35 +1174,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 3" xfId="1" xr:uid="{3EB3DAA0-9F71-48CB-8FEA-1E1CAF40E04C}"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -1311,9 +1280,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1351,7 +1320,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1457,7 +1426,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1599,7 +1568,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1691,7 +1660,7 @@
   <dimension ref="A1:D116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1704,13 +1673,27 @@
         <v>91</v>
       </c>
       <c r="B1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C1" t="s">
         <v>261</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>262</v>
       </c>
-      <c r="D1" t="s">
-        <v>263</v>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3227,7 +3210,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B111">
         <v>0.35</v>
@@ -3241,7 +3224,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B112">
         <v>0.21</v>
@@ -3269,7 +3252,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B114">
         <v>7.14</v>
@@ -3297,7 +3280,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B116">
         <v>286</v>
@@ -3311,7 +3294,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D116">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3324,7 +3307,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3342,22 +3325,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>279</v>
-      </c>
       <c r="F1" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>157</v>
@@ -3375,37 +3358,68 @@
         <v>136</v>
       </c>
       <c r="L1" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>282</v>
-      </c>
       <c r="O1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8">
+        <v>0</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8">
+        <v>0</v>
+      </c>
+      <c r="M2" s="8">
+        <v>0</v>
+      </c>
+      <c r="N2" s="8">
+        <v>0</v>
+      </c>
+      <c r="O2" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B3" s="8">
         <v>0</v>
@@ -3438,7 +3452,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M3" s="8">
         <v>1</v>
@@ -3452,7 +3466,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B4" s="8">
         <v>0</v>
@@ -3485,7 +3499,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M4" s="8">
         <v>1</v>
@@ -3499,7 +3513,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B5" s="8">
         <v>0</v>
@@ -3532,7 +3546,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M5" s="8">
         <v>1</v>
@@ -3546,7 +3560,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B6" s="8">
         <v>0</v>
@@ -3579,7 +3593,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M6" s="8">
         <v>1</v>
@@ -3593,7 +3607,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -3626,7 +3640,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M7" s="8">
         <v>1</v>
@@ -3640,7 +3654,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -3673,7 +3687,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M8" s="8">
         <v>0</v>
@@ -3687,7 +3701,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B9" s="8">
         <v>0</v>
@@ -3720,7 +3734,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M9" s="8">
         <v>1</v>
@@ -3734,7 +3748,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B10" s="8">
         <v>0</v>
@@ -3767,7 +3781,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M10" s="8">
         <v>1</v>
@@ -3781,7 +3795,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B11" s="8">
         <v>0</v>
@@ -3814,7 +3828,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M11" s="8">
         <v>1</v>
@@ -3828,7 +3842,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B12" s="8">
         <v>0</v>
@@ -3861,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M12" s="8">
         <v>1</v>
@@ -3875,7 +3889,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B13" s="8">
         <v>0</v>
@@ -3908,7 +3922,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M13" s="8">
         <v>1</v>
@@ -3922,7 +3936,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B14" s="8">
         <v>0</v>
@@ -3955,7 +3969,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M14" s="8">
         <v>1</v>
@@ -3969,7 +3983,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B15" s="8">
         <v>1</v>
@@ -4002,7 +4016,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M15" s="8">
         <v>1</v>
@@ -4016,7 +4030,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B16" s="8">
         <v>0</v>
@@ -4049,7 +4063,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M16" s="8">
         <v>1</v>
@@ -4063,7 +4077,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B17" s="8">
         <v>0</v>
@@ -4096,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M17" s="8">
         <v>1</v>
@@ -4110,7 +4124,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B18" s="8">
         <v>0</v>
@@ -4143,7 +4157,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M18" s="8">
         <v>1</v>
@@ -4157,7 +4171,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B19" s="8">
         <v>0</v>
@@ -4190,7 +4204,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M19" s="8">
         <v>1</v>
@@ -4204,7 +4218,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B20" s="8">
         <v>0</v>
@@ -4237,7 +4251,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M20" s="8">
         <v>1</v>
@@ -4251,7 +4265,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B21" s="8">
         <v>0</v>
@@ -4284,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M21" s="8">
         <v>1</v>
@@ -4298,7 +4312,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B22" s="8">
         <v>0</v>
@@ -4331,7 +4345,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M22" s="8">
         <v>1</v>
@@ -4345,7 +4359,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -4378,7 +4392,7 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -4392,7 +4406,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4439,7 +4453,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -4486,7 +4500,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4532,12 +4546,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8">
+  <conditionalFormatting sqref="J7:J8">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4550,8 +4559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6075F4E-6449-42F6-B0A2-E3B463F49D3C}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4585,6 +4594,32 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
@@ -4665,7 +4700,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4691,7 +4726,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4717,7 +4752,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5107,7 +5142,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -5444,18 +5479,13 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:H5 B9:H22 F6 B24:H35">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+  <conditionalFormatting sqref="B3:H22">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:H6">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:H8">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+  <conditionalFormatting sqref="F6 B24:H35">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5469,7 +5499,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5508,11 +5538,37 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5541,7 +5597,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5570,7 +5626,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5599,7 +5655,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -6208,7 +6264,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B27" s="8">
         <v>1</v>
@@ -6237,7 +6293,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B28" s="8">
         <v>1</v>
@@ -6266,7 +6322,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B29" s="8">
         <v>1</v>
@@ -6295,16 +6351,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B30" s="8">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>325</v>
-      </c>
-      <c r="B30" s="8">
-        <v>1</v>
-      </c>
-      <c r="C30" s="8">
-        <v>1</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>326</v>
       </c>
       <c r="E30" s="11">
         <v>0</v>
@@ -6382,7 +6438,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B33" s="8">
         <v>1</v>
@@ -6391,7 +6447,7 @@
         <v>1</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E33" s="11">
         <v>1</v>
@@ -6411,7 +6467,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:I26 B31:I32">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6423,7 +6479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D5AF32-1322-42FA-A3FF-C17883258B40}">
   <dimension ref="A1:Z110"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
@@ -6503,52 +6559,52 @@
         <v>113</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>114</v>
       </c>
       <c r="Z1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="O2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="P2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="S2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="T2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="U2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="V2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="W2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="X2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Y2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Z2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -15192,13 +15248,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:N110">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3:Z110">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+  <conditionalFormatting sqref="A3:Z110">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15281,10 +15332,10 @@
         <v>114</v>
       </c>
       <c r="V1" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="W1" t="s">
         <v>319</v>
-      </c>
-      <c r="W1" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -15428,7 +15479,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:W3">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15440,8 +15491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865B2AF4-2CF4-4093-8D70-C931333F20A4}">
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AJ5" sqref="AJ5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15452,7 +15503,7 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B1" t="s">
         <v>157</v>
@@ -15545,32 +15596,128 @@
         <v>156</v>
       </c>
       <c r="AF1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AG1" t="s">
         <v>180</v>
       </c>
-      <c r="AG1" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>158</v>
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>159</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>160</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -15591,16 +15738,16 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
+        <v>160</v>
+      </c>
+      <c r="M3" t="s">
         <v>161</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>162</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>163</v>
-      </c>
-      <c r="O3" t="s">
-        <v>164</v>
       </c>
       <c r="P3">
         <v>0.18</v>
@@ -15659,19 +15806,19 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>165</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>166</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -15760,19 +15907,19 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>167</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>168</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -15861,7 +16008,7 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -15873,7 +16020,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -15894,16 +16041,16 @@
         <v>0</v>
       </c>
       <c r="L6" t="s">
+        <v>160</v>
+      </c>
+      <c r="M6" t="s">
         <v>161</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>162</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>163</v>
-      </c>
-      <c r="O6" t="s">
-        <v>164</v>
       </c>
       <c r="P6">
         <v>0.18</v>
@@ -15962,7 +16109,7 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -15974,7 +16121,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -16063,7 +16210,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AG7">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16076,8 +16223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB4EA7-D669-4B1E-9B4E-C2CB3560F5F3}">
   <dimension ref="A1:AN24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:X1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AH20" sqref="AH20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16089,43 +16236,43 @@
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" t="s">
         <v>171</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>172</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>173</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>174</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>175</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>176</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>177</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>178</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>179</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>180</v>
-      </c>
-      <c r="M1" t="s">
-        <v>181</v>
       </c>
       <c r="N1" t="s">
         <v>157</v>
@@ -16146,78 +16293,200 @@
         <v>136</v>
       </c>
       <c r="T1" t="s">
+        <v>181</v>
+      </c>
+      <c r="U1" t="s">
         <v>182</v>
       </c>
-      <c r="U1" t="s">
-        <v>183</v>
-      </c>
       <c r="V1" t="s">
+        <v>184</v>
+      </c>
+      <c r="W1" t="s">
         <v>185</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>186</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>187</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>188</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>189</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>190</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>191</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>192</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>193</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>194</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>195</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>196</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>197</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>198</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>199</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>200</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>201</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>202</v>
       </c>
-      <c r="AN1" t="s">
-        <v>203</v>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>204</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>205</v>
       </c>
       <c r="D3">
         <v>0.375</v>
@@ -16333,13 +16602,13 @@
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D4">
         <v>0.39</v>
@@ -16455,13 +16724,13 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D5">
         <v>0.92</v>
@@ -16577,13 +16846,13 @@
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>208</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>209</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -16634,10 +16903,10 @@
         <v>0</v>
       </c>
       <c r="T6" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="U6" t="s">
         <v>210</v>
-      </c>
-      <c r="U6" t="s">
-        <v>211</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -16699,13 +16968,13 @@
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -16756,10 +17025,10 @@
         <v>0</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="U7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -16821,13 +17090,13 @@
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -16878,10 +17147,10 @@
         <v>0</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="U8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -16943,13 +17212,13 @@
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -17000,10 +17269,10 @@
         <v>0</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="U9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -17065,13 +17334,13 @@
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -17187,13 +17456,13 @@
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D11">
         <v>0.78500000000000003</v>
@@ -17309,13 +17578,13 @@
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D12">
         <v>0.83</v>
@@ -17431,13 +17700,13 @@
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D13">
         <v>0.4</v>
@@ -17553,13 +17822,13 @@
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D14">
         <v>0.98</v>
@@ -17675,13 +17944,13 @@
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D15">
         <v>0.98</v>
@@ -17797,13 +18066,13 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D16">
         <v>0.98</v>
@@ -17919,13 +18188,13 @@
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D17">
         <v>0.92</v>
@@ -18041,13 +18310,13 @@
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -18098,10 +18367,10 @@
         <v>0</v>
       </c>
       <c r="T18" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="U18" t="s">
         <v>210</v>
-      </c>
-      <c r="U18" t="s">
-        <v>211</v>
       </c>
       <c r="V18">
         <v>0</v>
@@ -18163,13 +18432,13 @@
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D19">
         <v>0.35</v>
@@ -18285,13 +18554,13 @@
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D20">
         <v>0.35</v>
@@ -18407,13 +18676,13 @@
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D21">
         <v>0.92</v>
@@ -18529,13 +18798,13 @@
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D22">
         <v>0.9</v>
@@ -18651,13 +18920,13 @@
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D23">
         <v>0.89</v>
@@ -18773,13 +19042,13 @@
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D24">
         <v>0.92</v>
@@ -18895,7 +19164,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AN24">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18907,8 +19176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062F9C9F-EC6B-45A0-B400-3E864B701D31}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18918,19 +19187,19 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" t="s">
         <v>180</v>
-      </c>
-      <c r="E1" t="s">
-        <v>181</v>
       </c>
       <c r="F1" t="s">
         <v>157</v>
@@ -18951,63 +19220,146 @@
         <v>136</v>
       </c>
       <c r="L1" t="s">
+        <v>231</v>
+      </c>
+      <c r="M1" t="s">
         <v>232</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>233</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>234</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>235</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>236</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>237</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>238</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
+        <v>173</v>
+      </c>
+      <c r="U1" t="s">
+        <v>174</v>
+      </c>
+      <c r="V1" t="s">
+        <v>176</v>
+      </c>
+      <c r="W1" t="s">
+        <v>177</v>
+      </c>
+      <c r="X1" t="s">
         <v>239</v>
       </c>
-      <c r="T1" t="s">
-        <v>174</v>
-      </c>
-      <c r="U1" t="s">
-        <v>175</v>
-      </c>
-      <c r="V1" t="s">
-        <v>177</v>
-      </c>
-      <c r="W1" t="s">
-        <v>178</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA1" t="s">
         <v>240</v>
       </c>
-      <c r="Y1" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>185</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>241</v>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>242</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>243</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -19084,13 +19436,13 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -19167,13 +19519,13 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -19250,13 +19602,13 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -19333,13 +19685,13 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -19416,13 +19768,13 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -19499,7 +19851,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:AA8">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19512,7 +19864,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19522,28 +19874,28 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" t="s">
         <v>180</v>
-      </c>
-      <c r="H1" t="s">
-        <v>181</v>
       </c>
       <c r="I1" t="s">
         <v>157</v>
@@ -19564,15 +19916,59 @@
         <v>136</v>
       </c>
     </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>251</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>252</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -19610,13 +20006,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -19654,13 +20050,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -19698,13 +20094,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -19742,13 +20138,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -19786,13 +20182,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -19830,13 +20226,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -19874,13 +20270,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D10">
         <v>0.9</v>
@@ -19918,13 +20314,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -19962,13 +20358,13 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -20006,13 +20402,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -20050,13 +20446,13 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -20094,13 +20490,13 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -20138,13 +20534,13 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -20182,13 +20578,13 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -20226,13 +20622,13 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -20270,13 +20666,13 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -20314,13 +20710,13 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -20358,22 +20754,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:N18">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:N20">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:N19">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20:C20">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20:N20">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>